<commit_message>
Update azure-pipelines-1.yml for Azure Pipelines
</commit_message>
<xml_diff>
--- a/DocumentProcessing/Output/DataTable.xlsx
+++ b/DocumentProcessing/Output/DataTable.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <x:si>
     <x:t>nom</x:t>
   </x:si>
@@ -64,46 +64,46 @@
     <x:t>A3536444</x:t>
   </x:si>
   <x:si>
-    <x:t>Viren V. Timbadiya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+91)(9909198882</x:t>
-  </x:si>
-  <x:si>
-    <x:t>viren0312@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>L/401 - Vrajdarshan Residency, Vraj Chowk, Simada, Surat - 395010 Gujarat, INDIA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diploma Pharmacy and Degree Pharmacy with Second Class from SAURASTRA UNIVERSITY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MBA in Marketing Specialization</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product Specialist at Johnson &amp; Johnson Medical (JJHS - Project handling by Medi Transcare Pvt Ltd) and Professional Service Representative at MsGlobus Remedies Ltd</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Name: Thajunnisa P H </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Phone Number: 9072048062 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Email: thajunnisaph@gmail.com </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Address: Pulinganal (H) Randar P.O Muvattupuzha Ernakulam, 686673 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Education: B-TECH Indira Gandhi Institute of Engineering and Technology for Women MG University 2016 Electronics &amp; Communication Engineering 7.51*/10 CGPA </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Skills: Skilled in understanding SRS and identifying the required test scenarios, Knowledge of writing Test Cases and Test Report, Good knowledge in automated tool like QTP, Knowledge in Unit, Integration and System Testing </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Experience: SOFTWARE TESTING course in Spyrosys</x:t>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phone number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Adress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Education</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Skills</x:t>
+  </x:si>
+  <x:si>
+    <x:t>expirience</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Chirine Bouzouita </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> +216 58300114 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> chirine.bouzouita@Sinorfi.com </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Sinorfi </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Diplôme d'Ingénieur en Informatique Industrielle </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Rédiger les documents de spécifications techniques et/ou fonctionnelles, Modéliser des données et mettre à jour la documentation technique, Paramétrage des profils Salesforce, Implémentation des classes Apex, Mise en place des composants LWC, Migration du Process Builder vers le Flow Builder, Réalisation des Tests, Maintenance corrective et évolutive, Santé </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> TALAN TUNISIE Consultante Technique Salesforce, Août 2022 - Juin 2023, Crosstalant, Intégration d'une application des gestions des ressources humaines, Stagiaire Consultante Salesforce (Projet de fin d'étude)</x:t>
   </x:si>
   <x:si>
     <x:t>Himanshu Tripathi</x:t>
@@ -190,25 +190,28 @@
     <x:t xml:space="preserve"> Vocational Summer training in BHEL Heavy Equipment Repair Plant Varanasi</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Chirine Bouzouita </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> +216 58300114 </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> chirine.bouzouita@Sinorfi.com </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Sinorfi </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Diplôme d'Ingénieur en Informatique Industrielle </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Rédiger les documents de spécifications techniques et/ou fonctionnelles, Modéliser des données et mettre à jour la documentation technique, Paramétrage des profils Salesforce, Implémentation des classes Apex, Mise en place des composants LWC, Migration du Process Builder vers le Flow Builder, Réalisation des Tests, Maintenance corrective et évolutive, Santé </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> TALAN TUNISIE Consultante Technique Salesforce, Août 2022 - Juin 2023, Crosstalant, Intégration d'une application des gestions des ressources humaines, Stagiaire Consultante Salesforce (Projet de fin d'étude)</x:t>
+    <x:t>Gouadria Oumaima</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+21693344006</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Go2u1a6d9ri3a@esprit.tn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 Rue 4359 Ezzouhour 5, Tunis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-Présent Ecole supérieure privée d'ingénierie et de technologies Cycle d'ingénieur en génie logiciel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Java/SpringBoot/node.js/JavaFx /CodenameOne /Agular/Python Angular/Symfony 3/ php5/Asp.net/ C# Html5/Css/Bootstrap/JavaScript/jQuery Web Service : REST/ SOAP /Git /Maven MySQL/SQL Server /Oracle /PLSQL Linux (CentOS/Ubuntu) Amazon S3, cloud front, RDS / Jenkins / Technologies utilisés : Jenkins/Github/nexus/ SonarQube/ Docker Compose /prometheus/graphana Doker /Git</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pidev 4W4 (Women for the Win) 02/2022 - 05/2022 Pidev Cyber Doc 02/2021 - 05/2021 Projet DevOps 09/2022 - 11/2022 Stage d'ingenieur juin 2022 - out 2022 Rhis Software Stage d'immersion en entreprise Out 2021 Attijari Bank Stage de PFE janvier 2020 - Juillet 2020 ADDIXO</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> TALAN TUNISIE Consultante Technique Salesforce, Août 2022 - Juin 2023, Crosstalant, ALBEA</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -562,7 +565,7 @@
       <x:selection activeCell="D2" sqref="D2"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="13.038125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="18.723125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
     <x:col min="1" max="2" width="10.179688" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="22.179688" style="0" customWidth="1"/>
@@ -855,25 +858,94 @@
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="A7" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="A8" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
+      <x:c r="B8" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="C8" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="D8" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="E7" s="0" t="s">
+      <x:c r="E8" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="F7" s="0" t="s">
+      <x:c r="F8" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="G7" s="0" t="s">
+      <x:c r="G8" s="0" t="s">
         <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:7">
+      <x:c r="A9" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:7">
+      <x:c r="A10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>